<commit_message>
AutoCommit_17 июня 2024 г. 19:48:11_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-722_ТерВер.xlsx
+++ b/2ИСИП-722_ТерВер.xlsx
@@ -554,10 +554,10 @@
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J26" sqref="J26"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -619,15 +619,9 @@
       <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="H3" s="1">
-        <v>1</v>
-      </c>
-      <c r="I3" s="8">
-        <v>1</v>
-      </c>
-      <c r="J3" s="8">
-        <v>1</v>
-      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -649,20 +643,20 @@
         <v>5</v>
       </c>
       <c r="G4" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H4" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I4" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J4" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L4">
         <f>SUM(C4:J4)</f>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="M4" s="7">
         <v>4</v>
@@ -730,17 +724,17 @@
         <v>5</v>
       </c>
       <c r="H6" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I6" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J6" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L6">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="M6" s="7">
         <v>4</v>
@@ -754,32 +748,32 @@
         <v>4</v>
       </c>
       <c r="C7" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D7" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E7" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F7" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G7" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H7" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I7" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J7" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M7" s="7">
         <v>3</v>
@@ -805,20 +799,20 @@
         <v>5</v>
       </c>
       <c r="G8" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H8" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I8" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J8" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="M8" s="7">
         <v>4</v>
@@ -853,11 +847,11 @@
         <v>5</v>
       </c>
       <c r="J9" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L9">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M9" s="7">
         <v>5</v>
@@ -928,14 +922,14 @@
         <v>5</v>
       </c>
       <c r="I11" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J11" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L11">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="M11" s="7">
         <v>5</v>
@@ -1045,14 +1039,14 @@
         <v>5</v>
       </c>
       <c r="I14" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J14" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L14">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="M14" s="7">
         <v>5</v>
@@ -1084,14 +1078,14 @@
         <v>5</v>
       </c>
       <c r="I15" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J15" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L15">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="M15" s="7">
         <v>5</v>
@@ -1144,32 +1138,32 @@
         <v>14</v>
       </c>
       <c r="C17" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D17" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E17" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F17" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G17" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H17" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I17" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J17" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M17" s="7">
         <v>3</v>
@@ -1195,20 +1189,20 @@
         <v>5</v>
       </c>
       <c r="G18" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H18" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I18" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J18" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L18">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="M18" s="7">
         <v>4</v>
@@ -1234,20 +1228,20 @@
         <v>5</v>
       </c>
       <c r="G19" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H19" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I19" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J19" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L19">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="M19" s="7">
         <v>4</v>
@@ -1300,32 +1294,32 @@
         <v>18</v>
       </c>
       <c r="C21" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D21" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E21" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F21" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G21" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H21" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I21" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J21" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M21" s="7">
         <v>3</v>
@@ -1384,26 +1378,26 @@
         <v>5</v>
       </c>
       <c r="E23" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F23" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G23" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H23" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I23" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J23" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L23">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="M23" s="7">
         <v>3</v>
@@ -1477,11 +1471,11 @@
         <v>5</v>
       </c>
       <c r="J25" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L25">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M25" s="7">
         <v>5</v>
@@ -1498,32 +1492,32 @@
         <v>23</v>
       </c>
       <c r="C26" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D26" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E26" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F26" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G26" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H26" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I26" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J26" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M26" s="7">
         <v>3</v>
@@ -1576,32 +1570,32 @@
         <v>25</v>
       </c>
       <c r="C28" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D28" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E28" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F28" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G28" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H28" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I28" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J28" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M28" s="7">
         <v>3</v>
@@ -1636,11 +1630,11 @@
         <v>5</v>
       </c>
       <c r="J29" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L29">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M29" s="7">
         <v>5</v>
@@ -1654,32 +1648,32 @@
         <v>27</v>
       </c>
       <c r="C30" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D30" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E30" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F30" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G30" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H30" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I30" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J30" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M30" s="7">
         <v>3</v>
@@ -1714,11 +1708,11 @@
         <v>4</v>
       </c>
       <c r="J31" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L31">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M31" s="7">
         <v>3</v>
@@ -1741,7 +1735,7 @@
         <v>5</v>
       </c>
       <c r="E32" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F32" s="2">
         <v>5</v>
@@ -1753,14 +1747,14 @@
         <v>5</v>
       </c>
       <c r="I32" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J32" s="6">
         <v>5</v>
       </c>
       <c r="L32">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="M32" s="7">
         <v>5</v>

</xml_diff>

<commit_message>
AutoCommit_17 июня 2024 г. 19:54:48_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-722_ТерВер.xlsx
+++ b/2ИСИП-722_ТерВер.xlsx
@@ -557,7 +557,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -619,9 +619,15 @@
       <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="8">
+        <v>1</v>
+      </c>
+      <c r="J3" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">

</xml_diff>

<commit_message>
AutoCommit_17 июня 2024 г. 20:00:51_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-722_ТерВер.xlsx
+++ b/2ИСИП-722_ТерВер.xlsx
@@ -557,7 +557,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
+      <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1702,7 +1702,7 @@
         <v>5</v>
       </c>
       <c r="F31" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G31" s="2">
         <v>4</v>
@@ -1718,10 +1718,10 @@
       </c>
       <c r="L31">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="M31" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O31" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
AutoCommit_19 июня 2024 г. 11:42:05_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-722_ТерВер.xlsx
+++ b/2ИСИП-722_ТерВер.xlsx
@@ -557,7 +557,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomRight" activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1234,23 +1234,23 @@
         <v>5</v>
       </c>
       <c r="G19" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H19" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I19" s="6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J19" s="7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L19">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="M19" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AutoCommit_20 июня 2024 г. 11:42:47_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-722_ТерВер.xlsx
+++ b/2ИСИП-722_ТерВер.xlsx
@@ -554,10 +554,10 @@
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O19" sqref="O19"/>
+      <selection pane="bottomRight" activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1498,32 +1498,32 @@
         <v>23</v>
       </c>
       <c r="C26" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D26" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E26" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F26" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G26" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H26" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I26" s="6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J26" s="7">
         <v>2</v>
       </c>
       <c r="L26">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="M26" s="7">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_20 июня 2024 г. 11:43:45_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-722_ТерВер.xlsx
+++ b/2ИСИП-722_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>2ИСИП-722: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -557,7 +557,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H26" sqref="H26"/>
+      <selection pane="bottomRight" activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1526,7 +1526,10 @@
         <v>37</v>
       </c>
       <c r="M26" s="7">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="N26" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AutoCommit_20 июня 2024 г. 12:35:04_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-722_ТерВер.xlsx
+++ b/2ИСИП-722_ТерВер.xlsx
@@ -554,10 +554,10 @@
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N26" sqref="N26"/>
+      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
AutoCommit_23 июня 2024 г. 20:08:15_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-722_ТерВер.xlsx
+++ b/2ИСИП-722_ТерВер.xlsx
@@ -560,7 +560,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="P4" sqref="P4:P32"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -625,21 +625,11 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1">
-        <v>1</v>
-      </c>
-      <c r="I3" s="8">
-        <v>1</v>
-      </c>
-      <c r="J3" s="8">
-        <v>1</v>
-      </c>
-      <c r="M3" s="9">
-        <v>1</v>
-      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="M3" s="9"/>
     </row>
     <row r="4" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">

</xml_diff>